<commit_message>
first cut of interruptible FLASH
</commit_message>
<xml_diff>
--- a/src/main/resources/devices/wokwi/Referees.xlsx
+++ b/src/main/resources/devices/wokwi/Referees.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms-firmata\src\main\resources\devices\biy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms-firmata\src\main\resources\devices\wokwi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92240AFC-E0EB-4DB1-AF74-2DD548F6A618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3186C64F-6078-45CE-B428-A4B7983B99BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
   <si>
     <t>pin</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>ignore A5</t>
+  </si>
+  <si>
+    <t>1000 200 200 6,7</t>
+  </si>
+  <si>
+    <t>1000 200 200 10,11</t>
+  </si>
+  <si>
+    <t>4000 200 200 2,3</t>
   </si>
 </sst>
 </file>
@@ -616,7 +625,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,7 +636,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -690,7 +699,7 @@
         <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -835,7 +844,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="7"/>
@@ -1011,7 +1020,7 @@
         <v>26</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:9">

</xml_diff>